<commit_message>
Removed extra files. Needs testing and updated products sheet
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -91,12 +91,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,10 +293,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -949,10 +953,18 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
+      <c r="A82" s="2" t="n">
         <v>12583241</v>
       </c>
       <c r="B82" s="0" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>12583189</v>
+      </c>
+      <c r="B83" s="0" t="n">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on selecting 20 random locations for counts
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usgarretan2\Downloads\Easy Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAFBA4C-3D34-4492-A2A5-33CA13FD7A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB984B24-47B9-406F-B2FC-9F998F445CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5231EC94-5F99-4FCD-B062-71A2B22C17ED}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FC85C5-C3A4-4AF5-8B01-C8731B21BBDA}">
-  <dimension ref="A1:B161"/>
+  <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,6 +1685,22 @@
       </c>
       <c r="B161">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>12600935</v>
+      </c>
+      <c r="B162">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>12613955</v>
+      </c>
+      <c r="B163">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>